<commit_message>
Included Winkler data for GE, CL, R and ca-cv
</commit_message>
<xml_diff>
--- a/experimental_data/GEC/Winkler1965.xlsx
+++ b/experimental_data/GEC/Winkler1965.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="39">
   <si>
     <t>Winkler1965 – Determination of hepatic flow in man</t>
   </si>
@@ -26,6 +26,9 @@
     <t>status</t>
   </si>
   <si>
+    <t>sample</t>
+  </si>
+  <si>
     <t>subject</t>
   </si>
   <si>
@@ -50,13 +53,10 @@
     <t>amount galactose infused [mmol/min]</t>
   </si>
   <si>
-    <t>hepatic blood flow [ml/min] M1</t>
-  </si>
-  <si>
-    <t>hepatic blood flow [ml/min] M2</t>
-  </si>
-  <si>
-    <t>hepatic blood flow [ml/min]</t>
+    <t>hepatic blood flow Bromsulfalein [ml/min]</t>
+  </si>
+  <si>
+    <t>hepatic blood flow galactose [ml/min]</t>
   </si>
   <si>
     <t>arterial concentrations galactose [mg/l]</t>
@@ -65,13 +65,16 @@
     <t>arterial concentrations galactose [mmol/l]</t>
   </si>
   <si>
-    <t>Arterio-hepatovenous extraction (per cent) M1</t>
-  </si>
-  <si>
-    <t>Arterio-hepatovenous extraction (per cent) M2</t>
-  </si>
-  <si>
-    <t>GE estimate: R = I – (DeltaP x V) [mmol/min]</t>
+    <t>Galactose arterio-hepatovenous extraction [percent]</t>
+  </si>
+  <si>
+    <t>Galactose extraction ratio [-]</t>
+  </si>
+  <si>
+    <t>Galactose clearance ER*Q [ml/min]</t>
+  </si>
+  <si>
+    <t>venous concentration galactose (1-ER)*ca [mmol/l]</t>
   </si>
   <si>
     <t>height</t>
@@ -89,10 +92,10 @@
     <t>galInfused</t>
   </si>
   <si>
-    <t>bloodflowM1</t>
-  </si>
-  <si>
-    <t>bloodflowM2</t>
+    <t>bloodflowBS</t>
+  </si>
+  <si>
+    <t>bloodflowGal</t>
   </si>
   <si>
     <t>flowLiver</t>
@@ -101,16 +104,19 @@
     <t>galAmg</t>
   </si>
   <si>
-    <t>galA</t>
-  </si>
-  <si>
-    <t>extractionM1</t>
-  </si>
-  <si>
-    <t>extractionM2</t>
-  </si>
-  <si>
-    <t>GEC</t>
+    <t>ca</t>
+  </si>
+  <si>
+    <t>extraction</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>cv</t>
   </si>
   <si>
     <t>win1965</t>
@@ -126,12 +132,6 @@
   </si>
   <si>
     <t>female</t>
-  </si>
-  <si>
-    <t>Measurements by indirect method of Bradley</t>
-  </si>
-  <si>
-    <t>S.D [%] 7</t>
   </si>
 </sst>
 </file>
@@ -179,7 +179,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,12 +196,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF999999"/>
         <bgColor rgb="FF808080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF9900"/>
-        <bgColor rgb="FFFFCC00"/>
       </patternFill>
     </fill>
     <fill>
@@ -245,7 +239,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -266,19 +260,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -359,15 +345,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>152280</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>136800</xdr:rowOff>
+      <xdr:colOff>147960</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>81720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>667800</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>116640</xdr:rowOff>
+      <xdr:colOff>663120</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>34560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -382,8 +368,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="152280" y="3103200"/>
-          <a:ext cx="2953800" cy="3204360"/>
+          <a:off x="147960" y="4889880"/>
+          <a:ext cx="2953440" cy="3204000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -398,15 +384,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>803520</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>82440</xdr:rowOff>
+      <xdr:colOff>809640</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>77760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>397800</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>26280</xdr:rowOff>
+      <xdr:colOff>740880</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>157320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -421,8 +407,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3241800" y="3048840"/>
-          <a:ext cx="3195360" cy="6094440"/>
+          <a:off x="3247920" y="4885920"/>
+          <a:ext cx="3195000" cy="6094080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -437,15 +423,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>485640</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>20520</xdr:rowOff>
+      <xdr:colOff>922680</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>139320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>153360</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:colOff>136800</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>117360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -460,8 +446,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6525000" y="3140640"/>
-          <a:ext cx="5402520" cy="5017680"/>
+          <a:off x="6624720" y="5109840"/>
+          <a:ext cx="5402160" cy="5017320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -481,26 +467,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5:B11"/>
+      <selection pane="topLeft" activeCell="T14" activeCellId="0" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.2959183673469"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.0357142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.4285714285714"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="14.3265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6989795918367"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.2959183673469"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.0357142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.4285714285714"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.4540816326531"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="14.3265306122449"/>
+    <col collapsed="false" hidden="false" max="18" min="16" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,6 +497,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
@@ -550,598 +540,1169 @@
         <v>13</v>
       </c>
       <c r="N2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" s="6" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="T2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" s="5" customFormat="true" ht="13.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="Q3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="R3" s="4" t="s">
         <v>31</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="0" t="n">
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="G4" s="0" t="n">
         <v>173</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="H4" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="H4" s="0" t="n">
-        <v>35</v>
-      </c>
       <c r="I4" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="J4" s="0" t="n">
         <v>211</v>
       </c>
-      <c r="J4" s="7" t="n">
-        <f aca="false">I4/180</f>
+      <c r="K4" s="6" t="n">
+        <f aca="false">J4/180</f>
         <v>1.17222222222222</v>
       </c>
-      <c r="K4" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>35</v>
+      <c r="L4" s="0" t="n">
+        <v>2040</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <f aca="false">L4</f>
+        <v>2040</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="G5" s="0" t="n">
         <v>182</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="H5" s="0" t="n">
         <v>81</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="I5" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="J5" s="0" t="n">
         <v>223</v>
       </c>
-      <c r="J5" s="7" t="n">
-        <f aca="false">I5/180</f>
+      <c r="K5" s="6" t="n">
+        <f aca="false">J5/180</f>
         <v>1.23888888888889</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="L5" s="0" t="n">
+        <v>2430</v>
+      </c>
+      <c r="M5" s="0" t="n">
         <v>2390</v>
       </c>
-      <c r="L5" s="0" t="n">
-        <v>2600</v>
-      </c>
-      <c r="M5" s="0" t="n">
-        <f aca="false">0.5*(K5+L5)</f>
-        <v>2495</v>
-      </c>
       <c r="N5" s="0" t="n">
+        <f aca="false">L5</f>
+        <v>2430</v>
+      </c>
+      <c r="O5" s="0" t="n">
         <v>152</v>
       </c>
-      <c r="O5" s="7" t="n">
-        <f aca="false">N5/180</f>
+      <c r="P5" s="6" t="n">
+        <f aca="false">O5/180</f>
         <v>0.844444444444444</v>
       </c>
-      <c r="P5" s="0" t="n">
+      <c r="Q5" s="0" t="n">
         <v>81.6</v>
       </c>
-      <c r="Q5" s="0" t="n">
-        <v>71.7</v>
-      </c>
       <c r="R5" s="0" t="n">
-        <f aca="false">0.5/100*(Q5+P5)*O5*0.5/1000*(K5+L5)</f>
-        <v>1.61493033333333</v>
+        <f aca="false">Q5/100</f>
+        <v>0.816</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <f aca="false"> R5*N5</f>
+        <v>1982.88</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <f aca="false">(1-R5)*P5</f>
+        <v>0.155377777777778</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="G6" s="0" t="n">
         <v>164</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="H6" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="H6" s="0" t="n">
-        <v>35</v>
-      </c>
       <c r="I6" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="J6" s="0" t="n">
         <v>185</v>
       </c>
-      <c r="J6" s="7" t="n">
-        <f aca="false">I6/180</f>
+      <c r="K6" s="6" t="n">
+        <f aca="false">J6/180</f>
         <v>1.02777777777778</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="L6" s="0" t="n">
+        <v>2180</v>
+      </c>
+      <c r="M6" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="L6" s="0" t="n">
-        <v>2250</v>
-      </c>
-      <c r="M6" s="0" t="n">
-        <f aca="false">0.5*(K6+L6)</f>
-        <v>2125</v>
-      </c>
       <c r="N6" s="0" t="n">
+        <f aca="false">L6</f>
+        <v>2180</v>
+      </c>
+      <c r="O6" s="0" t="n">
         <v>161</v>
       </c>
-      <c r="O6" s="7" t="n">
-        <f aca="false">N6/180</f>
+      <c r="P6" s="6" t="n">
+        <f aca="false">O6/180</f>
         <v>0.894444444444444</v>
       </c>
-      <c r="P6" s="0" t="n">
+      <c r="Q6" s="0" t="n">
         <v>65.8</v>
       </c>
-      <c r="Q6" s="0" t="n">
-        <v>58.4</v>
-      </c>
       <c r="R6" s="0" t="n">
-        <f aca="false">0.5/100*(Q6+P6)*O6*0.5/1000*(K6+L6)</f>
-        <v>1.18033125</v>
+        <f aca="false">Q6/100</f>
+        <v>0.658</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <f aca="false"> R6*N6</f>
+        <v>1434.44</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <f aca="false">(1-R6)*P6</f>
+        <v>0.3059</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="G7" s="0" t="n">
         <v>160</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="H7" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="I7" s="0" t="n">
         <v>58</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="J7" s="0" t="n">
         <v>267</v>
       </c>
-      <c r="J7" s="7" t="n">
-        <f aca="false">I7/180</f>
+      <c r="K7" s="6" t="n">
+        <f aca="false">J7/180</f>
         <v>1.48333333333333</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="L7" s="0" t="n">
+        <v>1960</v>
+      </c>
+      <c r="M7" s="0" t="n">
         <v>1450</v>
       </c>
-      <c r="L7" s="0" t="n">
-        <v>1510</v>
-      </c>
-      <c r="M7" s="0" t="n">
-        <f aca="false">0.5*(K7+L7)</f>
-        <v>1480</v>
-      </c>
       <c r="N7" s="0" t="n">
+        <f aca="false">L7</f>
+        <v>1960</v>
+      </c>
+      <c r="O7" s="0" t="n">
         <v>346</v>
       </c>
-      <c r="O7" s="7" t="n">
-        <f aca="false">N7/180</f>
+      <c r="P7" s="6" t="n">
+        <f aca="false">O7/180</f>
         <v>1.92222222222222</v>
       </c>
-      <c r="P7" s="0" t="n">
+      <c r="Q7" s="0" t="n">
         <v>67.3</v>
       </c>
-      <c r="Q7" s="0" t="n">
-        <v>65.3</v>
-      </c>
       <c r="R7" s="0" t="n">
-        <f aca="false">0.5/100*(Q7+P7)*O7*0.5/1000*(K7+L7)</f>
-        <v>1.88616133333333</v>
+        <f aca="false">Q7/100</f>
+        <v>0.673</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <f aca="false"> R7*N7</f>
+        <v>1319.08</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <f aca="false">(1-R7)*P7</f>
+        <v>0.628566666666666</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="G8" s="0" t="n">
         <v>188</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="H8" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="I8" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="J8" s="0" t="n">
         <v>366</v>
       </c>
-      <c r="J8" s="7" t="n">
-        <f aca="false">I8/180</f>
+      <c r="K8" s="6" t="n">
+        <f aca="false">J8/180</f>
         <v>2.03333333333333</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="L8" s="0" t="n">
+        <v>1470</v>
+      </c>
+      <c r="M8" s="0" t="n">
         <v>1780</v>
       </c>
-      <c r="L8" s="0" t="n">
-        <v>1680</v>
-      </c>
-      <c r="M8" s="0" t="n">
-        <f aca="false">0.5*(K8+L8)</f>
-        <v>1730</v>
-      </c>
       <c r="N8" s="0" t="n">
+        <f aca="false">L8</f>
+        <v>1470</v>
+      </c>
+      <c r="O8" s="0" t="n">
         <v>271</v>
       </c>
-      <c r="O8" s="7" t="n">
-        <f aca="false">N8/180</f>
+      <c r="P8" s="6" t="n">
+        <f aca="false">O8/180</f>
         <v>1.50555555555556</v>
       </c>
-      <c r="P8" s="0" t="n">
+      <c r="Q8" s="0" t="n">
         <v>93</v>
       </c>
-      <c r="Q8" s="0" t="n">
-        <v>98.5</v>
-      </c>
       <c r="R8" s="0" t="n">
-        <f aca="false">0.5/100*(Q8+P8)*O8*0.5/1000*(K8+L8)</f>
-        <v>2.49391513888889</v>
+        <f aca="false">Q8/100</f>
+        <v>0.93</v>
+      </c>
+      <c r="S8" s="0" t="n">
+        <f aca="false"> R8*N8</f>
+        <v>1367.1</v>
+      </c>
+      <c r="T8" s="0" t="n">
+        <f aca="false">(1-R8)*P8</f>
+        <v>0.105388888888889</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="G9" s="0" t="n">
         <v>183</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="H9" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="I9" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="J9" s="0" t="n">
         <v>305</v>
       </c>
-      <c r="J9" s="7" t="n">
-        <f aca="false">I9/180</f>
+      <c r="K9" s="6" t="n">
+        <f aca="false">J9/180</f>
         <v>1.69444444444444</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="L9" s="0" t="n">
+        <v>1260</v>
+      </c>
+      <c r="M9" s="0" t="n">
         <v>1580</v>
       </c>
-      <c r="L9" s="0" t="n">
-        <v>1800</v>
-      </c>
-      <c r="M9" s="0" t="n">
-        <f aca="false">0.5*(K9+L9)</f>
-        <v>1690</v>
-      </c>
       <c r="N9" s="0" t="n">
+        <f aca="false">L9</f>
+        <v>1260</v>
+      </c>
+      <c r="O9" s="0" t="n">
         <v>294</v>
       </c>
-      <c r="O9" s="7" t="n">
-        <f aca="false">N9/180</f>
+      <c r="P9" s="6" t="n">
+        <f aca="false">O9/180</f>
         <v>1.63333333333333</v>
       </c>
-      <c r="P9" s="0" t="n">
+      <c r="Q9" s="0" t="n">
         <v>77.6</v>
       </c>
-      <c r="Q9" s="0" t="n">
-        <v>68.4</v>
-      </c>
       <c r="R9" s="0" t="n">
-        <f aca="false">0.5/100*(Q9+P9)*O9*0.5/1000*(K9+L9)</f>
-        <v>2.01504333333333</v>
+        <f aca="false">Q9/100</f>
+        <v>0.776</v>
+      </c>
+      <c r="S9" s="0" t="n">
+        <f aca="false"> R9*N9</f>
+        <v>977.76</v>
+      </c>
+      <c r="T9" s="0" t="n">
+        <f aca="false">(1-R9)*P9</f>
+        <v>0.365866666666666</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="G10" s="0" t="n">
         <v>159</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="H10" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="I10" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="J10" s="0" t="n">
         <v>269</v>
       </c>
-      <c r="J10" s="7" t="n">
-        <f aca="false">I10/180</f>
+      <c r="K10" s="6" t="n">
+        <f aca="false">J10/180</f>
         <v>1.49444444444444</v>
       </c>
-      <c r="K10" s="0" t="n">
+      <c r="L10" s="0" t="n">
+        <v>1440</v>
+      </c>
+      <c r="M10" s="0" t="n">
         <v>1450</v>
       </c>
-      <c r="L10" s="0" t="n">
-        <v>1730</v>
-      </c>
-      <c r="M10" s="0" t="n">
-        <f aca="false">0.5*(K10+L10)</f>
-        <v>1590</v>
-      </c>
       <c r="N10" s="0" t="n">
+        <f aca="false">L10</f>
+        <v>1440</v>
+      </c>
+      <c r="O10" s="0" t="n">
         <v>237</v>
       </c>
-      <c r="O10" s="7" t="n">
-        <f aca="false">N10/180</f>
+      <c r="P10" s="6" t="n">
+        <f aca="false">O10/180</f>
         <v>1.31666666666667</v>
       </c>
-      <c r="P10" s="0" t="n">
+      <c r="Q10" s="0" t="n">
         <v>92.8</v>
       </c>
-      <c r="Q10" s="0" t="n">
-        <v>78.1</v>
-      </c>
       <c r="R10" s="0" t="n">
-        <f aca="false">0.5/100*(Q10+P10)*O10*0.5/1000*(K10+L10)</f>
-        <v>1.78889575</v>
+        <f aca="false">Q10/100</f>
+        <v>0.928</v>
+      </c>
+      <c r="S10" s="0" t="n">
+        <f aca="false"> R10*N10</f>
+        <v>1336.32</v>
+      </c>
+      <c r="T10" s="0" t="n">
+        <f aca="false">(1-R10)*P10</f>
+        <v>0.0948000000000003</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="E11" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>171</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>287</v>
+      </c>
+      <c r="K11" s="6" t="n">
+        <f aca="false">J11/180</f>
+        <v>1.59444444444444</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>1410</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>1470</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <f aca="false">L11</f>
+        <v>1410</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>266</v>
+      </c>
+      <c r="P11" s="6" t="n">
+        <f aca="false">O11/180</f>
+        <v>1.47777777777778</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <v>85.3</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <f aca="false">Q11/100</f>
+        <v>0.853</v>
+      </c>
+      <c r="S11" s="0" t="n">
+        <f aca="false"> R11*N11</f>
+        <v>1202.73</v>
+      </c>
+      <c r="T11" s="0" t="n">
+        <f aca="false">(1-R11)*P11</f>
+        <v>0.217233333333334</v>
+      </c>
+    </row>
+    <row r="12" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="F12" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>173</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>211</v>
+      </c>
+      <c r="K12" s="6" t="n">
+        <f aca="false">J12/180</f>
+        <v>1.17222222222222</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>1900</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <f aca="false">L12</f>
+        <v>1900</v>
+      </c>
+      <c r="O12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="P12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="R12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="T12" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>182</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>223</v>
+      </c>
+      <c r="K13" s="6" t="n">
+        <f aca="false">J13/180</f>
+        <v>1.23888888888889</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>2420</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>2600</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <f aca="false">L13</f>
+        <v>2420</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>152</v>
+      </c>
+      <c r="P13" s="6" t="n">
+        <f aca="false">O13/180</f>
+        <v>0.844444444444444</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>71.7</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <f aca="false">Q13/100</f>
+        <v>0.717</v>
+      </c>
+      <c r="S13" s="0" t="n">
+        <f aca="false"> R13*N13</f>
+        <v>1735.14</v>
+      </c>
+      <c r="T13" s="0" t="n">
+        <f aca="false">(1-R13)*P13</f>
+        <v>0.238977777777778</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>164</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>185</v>
+      </c>
+      <c r="K14" s="6" t="n">
+        <f aca="false">J14/180</f>
+        <v>1.02777777777778</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>2780</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>2250</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <f aca="false">L14</f>
+        <v>2780</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>161</v>
+      </c>
+      <c r="P14" s="6" t="n">
+        <f aca="false">O14/180</f>
+        <v>0.894444444444444</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <v>58.4</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <f aca="false">Q14/100</f>
+        <v>0.584</v>
+      </c>
+      <c r="S14" s="0" t="n">
+        <f aca="false"> R14*N14</f>
+        <v>1623.52</v>
+      </c>
+      <c r="T14" s="0" t="n">
+        <f aca="false">(1-R14)*P14</f>
+        <v>0.372088888888889</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>160</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>267</v>
+      </c>
+      <c r="K15" s="6" t="n">
+        <f aca="false">J15/180</f>
+        <v>1.48333333333333</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>1480</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>1510</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <f aca="false">L15</f>
+        <v>1480</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>346</v>
+      </c>
+      <c r="P15" s="6" t="n">
+        <f aca="false">O15/180</f>
+        <v>1.92222222222222</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <v>65.3</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <f aca="false">Q15/100</f>
+        <v>0.653</v>
+      </c>
+      <c r="S15" s="0" t="n">
+        <f aca="false"> R15*N15</f>
+        <v>966.44</v>
+      </c>
+      <c r="T15" s="0" t="n">
+        <f aca="false">(1-R15)*P15</f>
+        <v>0.667011111111111</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>188</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="K16" s="6" t="n">
+        <f aca="false">J16/180</f>
+        <v>2.03333333333333</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>1460</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>1680</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <f aca="false">L16</f>
+        <v>1460</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>271</v>
+      </c>
+      <c r="P16" s="6" t="n">
+        <f aca="false">O16/180</f>
+        <v>1.50555555555556</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <v>98.5</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <f aca="false">Q16/100</f>
+        <v>0.985</v>
+      </c>
+      <c r="S16" s="0" t="n">
+        <f aca="false"> R16*N16</f>
+        <v>1438.1</v>
+      </c>
+      <c r="T16" s="0" t="n">
+        <f aca="false">(1-R16)*P16</f>
+        <v>0.0225833333333334</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>183</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>305</v>
+      </c>
+      <c r="K17" s="6" t="n">
+        <f aca="false">J17/180</f>
+        <v>1.69444444444444</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>1280</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>1800</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <f aca="false">L17</f>
+        <v>1280</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>294</v>
+      </c>
+      <c r="P17" s="6" t="n">
+        <f aca="false">O17/180</f>
+        <v>1.63333333333333</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <v>68.4</v>
+      </c>
+      <c r="R17" s="0" t="n">
+        <f aca="false">Q17/100</f>
+        <v>0.684</v>
+      </c>
+      <c r="S17" s="0" t="n">
+        <f aca="false"> R17*N17</f>
+        <v>875.52</v>
+      </c>
+      <c r="T17" s="0" t="n">
+        <f aca="false">(1-R17)*P17</f>
+        <v>0.516133333333333</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>159</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>269</v>
+      </c>
+      <c r="K18" s="6" t="n">
+        <f aca="false">J18/180</f>
+        <v>1.49444444444444</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>1230</v>
+      </c>
+      <c r="M18" s="0" t="n">
+        <v>1730</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <f aca="false">L18</f>
+        <v>1230</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <v>237</v>
+      </c>
+      <c r="P18" s="6" t="n">
+        <f aca="false">O18/180</f>
+        <v>1.31666666666667</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <v>78.1</v>
+      </c>
+      <c r="R18" s="0" t="n">
+        <f aca="false">Q18/100</f>
+        <v>0.781</v>
+      </c>
+      <c r="S18" s="0" t="n">
+        <f aca="false"> R18*N18</f>
+        <v>960.63</v>
+      </c>
+      <c r="T18" s="0" t="n">
+        <f aca="false">(1-R18)*P18</f>
+        <v>0.28835</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="G19" s="0" t="n">
         <v>171</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="H19" s="0" t="n">
         <v>56</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="I19" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="J19" s="0" t="n">
         <v>287</v>
       </c>
-      <c r="J11" s="7" t="n">
-        <f aca="false">I11/180</f>
+      <c r="K19" s="6" t="n">
+        <f aca="false">J19/180</f>
         <v>1.59444444444444</v>
       </c>
-      <c r="K11" s="0" t="n">
-        <v>1470</v>
-      </c>
-      <c r="L11" s="0" t="n">
+      <c r="L19" s="0" t="n">
+        <v>1100</v>
+      </c>
+      <c r="M19" s="0" t="n">
         <v>1430</v>
       </c>
-      <c r="M11" s="0" t="n">
-        <f aca="false">0.5*(K11+L11)</f>
-        <v>1450</v>
-      </c>
-      <c r="N11" s="0" t="n">
+      <c r="N19" s="0" t="n">
+        <f aca="false">L19</f>
+        <v>1100</v>
+      </c>
+      <c r="O19" s="0" t="n">
         <v>266</v>
       </c>
-      <c r="O11" s="7" t="n">
-        <f aca="false">N11/180</f>
+      <c r="P19" s="6" t="n">
+        <f aca="false">O19/180</f>
         <v>1.47777777777778</v>
       </c>
-      <c r="P11" s="0" t="n">
-        <v>85.3</v>
-      </c>
-      <c r="Q11" s="0" t="n">
+      <c r="Q19" s="0" t="n">
         <v>90.2</v>
       </c>
-      <c r="R11" s="0" t="n">
-        <f aca="false">0.5/100*(Q11+P11)*O11*0.5/1000*(K11+L11)</f>
-        <v>1.8802875</v>
-      </c>
-    </row>
-    <row r="12" s="7" customFormat="true" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G12" s="0"/>
-      <c r="H12" s="0"/>
-      <c r="I12" s="0"/>
-      <c r="J12" s="0"/>
-      <c r="K12" s="0"/>
-      <c r="L12" s="0"/>
-      <c r="M12" s="0"/>
-      <c r="N12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G14" s="8" t="n">
-        <f aca="false">SUM(I4:I11)/COUNT(I4:I11)</f>
-        <v>264.125</v>
-      </c>
-      <c r="H14" s="8" t="n">
-        <f aca="false">SUM(J4:J11)/COUNT(J4:J11)</f>
-        <v>1.46736111111111</v>
-      </c>
-      <c r="J14" s="8" t="n">
-        <f aca="false">SUM(K5:L11)/COUNT(K5:L11)</f>
-        <v>1794.28571428571</v>
-      </c>
-      <c r="K14" s="8" t="n">
-        <f aca="false">SUM(N4:N11)/COUNT(N4:N11)</f>
-        <v>246.714285714286</v>
-      </c>
-      <c r="M14" s="7"/>
-      <c r="N14" s="8" t="n">
-        <f aca="false">SUM(Q4:Q11)/COUNT(Q4:Q11)</f>
-        <v>75.8</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J15" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="R19" s="0" t="n">
+        <f aca="false">Q19/100</f>
+        <v>0.902</v>
+      </c>
+      <c r="S19" s="0" t="n">
+        <f aca="false"> R19*N19</f>
+        <v>992.2</v>
+      </c>
+      <c r="T19" s="0" t="n">
+        <f aca="false">(1-R19)*P19</f>
+        <v>0.144822222222222</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>